<commit_message>
improve report and program
</commit_message>
<xml_diff>
--- a/entropy.xlsx
+++ b/entropy.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18570" windowHeight="10850" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18570" windowHeight="10850" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Chart2" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$C$1</definedName>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="102">
   <si>
     <t>NaN</t>
   </si>
@@ -319,12 +321,30 @@
   </si>
   <si>
     <t>Mutual Information</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>error rate</t>
+  </si>
+  <si>
+    <t>minimum</t>
+  </si>
+  <si>
+    <t>k = 3</t>
+  </si>
+  <si>
+    <t>k = 23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -354,10 +374,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -770,11 +794,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="754912416"/>
-        <c:axId val="754913592"/>
+        <c:axId val="368535800"/>
+        <c:axId val="368541680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="754912416"/>
+        <c:axId val="368535800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -817,7 +841,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="754913592"/>
+        <c:crossAx val="368541680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -825,7 +849,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="754913592"/>
+        <c:axId val="368541680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -876,9 +900,998 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="754912416"/>
+        <c:crossAx val="368535800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>bug</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet2!$C$6:$C$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="11"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.02</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.02</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.01</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.05</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.06</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.06</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>7.0000000000000007E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>7.0000000000000007E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0.06</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>0.05</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet2!$C$6:$C$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="11"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.02</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.02</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.01</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.05</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.06</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.06</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>7.0000000000000007E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>7.0000000000000007E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0.06</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>0.05</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$6:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$6:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>suggestion</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="plus"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet2!$E$6:$E$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="11"/>
+                  <c:pt idx="0">
+                    <c:v>0.01</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.13</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.13</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.14000000000000001</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.04</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.24</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.17</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.22</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.21</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet2!$E$6:$E$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="11"/>
+                  <c:pt idx="0">
+                    <c:v>0.01</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.13</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.13</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.14000000000000001</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.04</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.24</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.17</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.22</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.21</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:srgbClr val="00B050"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$6:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$6:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>question</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:srgbClr val="00B0F0"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet2!$G$6:$G$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="11"/>
+                  <c:pt idx="0">
+                    <c:v>0.01</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.06</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.11</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.05</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.06</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.06</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0.19</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>0.24</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet2!$G$6:$G$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="11"/>
+                  <c:pt idx="0">
+                    <c:v>0.01</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.06</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.11</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.05</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.06</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.06</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0.19</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>0.24</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:srgbClr val="00B0F0"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$6:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$F$6:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="375093360"/>
+        <c:axId val="375093752"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="375093360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Minimum</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Mutual Information (bits)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="375093752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="375093752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.70000000000000007"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Error Rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="375093360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -979,6 +1992,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1482,6 +2535,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
@@ -1494,11 +3063,50 @@
 </chartsheet>
 </file>
 
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
     <xdr:ext cx="10200640" cy="7137400"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="10195034" cy="7133897"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1786,8 +3394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1823,9 +3431,9 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="2">
+        <v>22</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
@@ -1834,7 +3442,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
@@ -1845,7 +3453,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>0</v>
@@ -1859,7 +3467,7 @@
         <v>24</v>
       </c>
       <c r="B6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -1870,7 +3478,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
@@ -1880,65 +3488,65 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>0</v>
+        <v>49</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="C8">
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B9" s="2">
-        <v>0.81100000000000005</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="C9">
-        <v>0.73799999999999999</v>
+        <v>0.26400000000000001</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="C10">
-        <v>0.71399999999999997</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2">
-        <v>5.6000000000000001E-2</v>
+        <v>0.54700000000000004</v>
       </c>
       <c r="C11">
-        <v>0.629</v>
+        <v>-9.7000000000000003E-2</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2">
-        <v>0.08</v>
+        <v>0.53800000000000003</v>
       </c>
       <c r="C12">
-        <v>0.54600000000000004</v>
+        <v>-6.9000000000000006E-2</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="2" t="s">
@@ -1953,13 +3561,13 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="B13" s="2">
-        <v>9.0999999999999998E-2</v>
+        <v>0.51600000000000001</v>
       </c>
       <c r="C13">
-        <v>0.497</v>
+        <v>-0.111</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
@@ -1974,13 +3582,13 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="B14" s="2">
-        <v>9.8000000000000004E-2</v>
+        <v>0.48399999999999999</v>
       </c>
       <c r="C14">
-        <v>0.48099999999999998</v>
+        <v>-0.11899999999999999</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
@@ -1995,13 +3603,13 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B15" s="2">
-        <v>9.5000000000000001E-2</v>
+        <v>0.48</v>
       </c>
       <c r="C15">
-        <v>0.47699999999999998</v>
+        <v>-0.13</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
@@ -2019,10 +3627,10 @@
         <v>34</v>
       </c>
       <c r="B16" s="2">
-        <v>0.111</v>
+        <v>0.47199999999999998</v>
       </c>
       <c r="C16">
-        <v>0.433</v>
+        <v>-0.13200000000000001</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
@@ -2037,13 +3645,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B17" s="2">
-        <v>0.75</v>
+        <v>0.47099999999999997</v>
       </c>
       <c r="C17">
-        <v>0.40799999999999997</v>
+        <v>-0.13900000000000001</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
@@ -2058,13 +3666,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="B18" s="2">
-        <v>0.14199999999999999</v>
+        <v>0.43099999999999999</v>
       </c>
       <c r="C18">
-        <v>0.35899999999999999</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
@@ -2079,13 +3687,13 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="B19" s="2">
-        <v>0.14099999999999999</v>
+        <v>0.42899999999999999</v>
       </c>
       <c r="C19">
-        <v>0.35</v>
+        <v>-0.14199999999999999</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
@@ -2100,13 +3708,13 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="B20" s="2">
-        <v>0.159</v>
+        <v>0.42699999999999999</v>
       </c>
       <c r="C20">
-        <v>0.29499999999999998</v>
+        <v>-0.14499999999999999</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
@@ -2121,13 +3729,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="B21" s="2">
-        <v>0.56000000000000005</v>
+        <v>0.41899999999999998</v>
       </c>
       <c r="C21">
-        <v>0.29399999999999998</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
@@ -2142,13 +3750,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B22" s="2">
-        <v>0.16900000000000001</v>
+        <v>0.41399999999999998</v>
       </c>
       <c r="C22">
-        <v>0.26300000000000001</v>
+        <v>-0.14499999999999999</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
@@ -2163,13 +3771,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="B23" s="2">
-        <v>0.17199999999999999</v>
+        <v>0.40400000000000003</v>
       </c>
       <c r="C23">
-        <v>0.25700000000000001</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
@@ -2184,13 +3792,13 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B24" s="2">
-        <v>0.65</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="C24">
-        <v>0.21299999999999999</v>
+        <v>-0.127</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
@@ -2205,13 +3813,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="B25" s="2">
-        <v>0.19400000000000001</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="C25">
-        <v>0.20499999999999999</v>
+        <v>-0.14499999999999999</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
@@ -2226,13 +3834,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="B26" s="2">
-        <v>0.216</v>
+        <v>0.38300000000000001</v>
       </c>
       <c r="C26">
-        <v>0.189</v>
+        <v>-0.14299999999999999</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
@@ -2247,13 +3855,13 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B27" s="2">
-        <v>0.20899999999999999</v>
+        <v>0.38200000000000001</v>
       </c>
       <c r="C27">
-        <v>0.17799999999999999</v>
+        <v>-0.14499999999999999</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
@@ -2268,13 +3876,13 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B28" s="2">
-        <v>0.20899999999999999</v>
+        <v>0.38</v>
       </c>
       <c r="C28">
-        <v>0.17100000000000001</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
@@ -2289,13 +3897,13 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B29" s="2">
-        <v>0.23799999999999999</v>
+        <v>0.379</v>
       </c>
       <c r="C29">
-        <v>0.13700000000000001</v>
+        <v>-0.14199999999999999</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>42</v>
@@ -2309,13 +3917,13 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="B30" s="2">
-        <v>0.23200000000000001</v>
+        <v>0.36699999999999999</v>
       </c>
       <c r="C30">
-        <v>0.13500000000000001</v>
+        <v>-0.12</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>13</v>
@@ -2329,13 +3937,13 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B31" s="2">
-        <v>0.23300000000000001</v>
+        <v>0.35199999999999998</v>
       </c>
       <c r="C31">
-        <v>0.13300000000000001</v>
+        <v>-0.114</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>10</v>
@@ -2349,13 +3957,13 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B32" s="2">
-        <v>0.253</v>
+        <v>0.34200000000000003</v>
       </c>
       <c r="C32">
-        <v>0.11700000000000001</v>
+        <v>-0.121</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>8</v>
@@ -2369,13 +3977,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B33" s="2">
-        <v>0.5</v>
+        <v>0.34</v>
       </c>
       <c r="C33">
-        <v>0.109</v>
+        <v>-0.13100000000000001</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>19</v>
@@ -2389,13 +3997,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B34" s="2">
-        <v>0.23599999999999999</v>
+        <v>0.33900000000000002</v>
       </c>
       <c r="C34">
-        <v>0.108</v>
+        <v>-0.111</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>17</v>
@@ -2409,13 +4017,13 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="B35" s="2">
-        <v>0.55800000000000005</v>
+        <v>0.33800000000000002</v>
       </c>
       <c r="C35">
-        <v>0.107</v>
+        <v>-0.11799999999999999</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>61</v>
@@ -2429,112 +4037,112 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="B36" s="2">
-        <v>0.53200000000000003</v>
+        <v>0.33800000000000002</v>
       </c>
       <c r="C36">
-        <v>9.8000000000000004E-2</v>
+        <v>-0.13700000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B37" s="2">
-        <v>0.25700000000000001</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="C37">
-        <v>9.8000000000000004E-2</v>
+        <v>-0.11899999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="B38" s="2">
-        <v>0.53300000000000003</v>
+        <v>0.32400000000000001</v>
       </c>
       <c r="C38">
-        <v>8.2000000000000003E-2</v>
+        <v>-0.107</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B39" s="2">
-        <v>0.54500000000000004</v>
+        <v>0.32</v>
       </c>
       <c r="C39">
-        <v>8.2000000000000003E-2</v>
+        <v>-0.104</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="B40" s="2">
-        <v>0.44400000000000001</v>
+        <v>0.316</v>
       </c>
       <c r="C40">
-        <v>8.2000000000000003E-2</v>
+        <v>-0.104</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="B41" s="2">
-        <v>0.54500000000000004</v>
+        <v>0.309</v>
       </c>
       <c r="C41">
-        <v>8.2000000000000003E-2</v>
+        <v>-0.10100000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="B42" s="2">
-        <v>0.27800000000000002</v>
+        <v>0.309</v>
       </c>
       <c r="C42">
-        <v>8.2000000000000003E-2</v>
+        <v>-0.10299999999999999</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="B43" s="2">
-        <v>0.54100000000000004</v>
+        <v>0.308</v>
       </c>
       <c r="C43">
-        <v>7.4999999999999997E-2</v>
+        <v>-9.8000000000000004E-2</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="B44" s="2">
-        <v>0.52700000000000002</v>
+        <v>0.30599999999999999</v>
       </c>
       <c r="C44">
-        <v>7.1999999999999995E-2</v>
+        <v>-9.7000000000000003E-2</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="B45" s="2">
-        <v>0.51700000000000002</v>
+        <v>0.29899999999999999</v>
       </c>
       <c r="C45">
-        <v>6.8000000000000005E-2</v>
+        <v>-0.09</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
@@ -2542,65 +4150,65 @@
         <v>6</v>
       </c>
       <c r="B46" s="2">
-        <v>0.54200000000000004</v>
+        <v>0.29199999999999998</v>
       </c>
       <c r="C46">
-        <v>6.6000000000000003E-2</v>
+        <v>-7.9000000000000001E-2</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B47" s="2">
-        <v>0.27600000000000002</v>
+        <v>0.29099999999999998</v>
       </c>
       <c r="C47">
-        <v>6.6000000000000003E-2</v>
+        <v>-8.2000000000000003E-2</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B48" s="2">
-        <v>0.28899999999999998</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="C48">
-        <v>6.2E-2</v>
+        <v>-8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="B49" s="2">
-        <v>0.51100000000000001</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C49">
-        <v>6.0999999999999999E-2</v>
+        <v>-5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B50" s="2">
-        <v>0.29499999999999998</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="C50">
-        <v>5.8000000000000003E-2</v>
+        <v>-5.6000000000000001E-2</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="B51" s="2">
-        <v>0.29899999999999999</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="C51">
-        <v>5.3999999999999999E-2</v>
+        <v>-9.6000000000000002E-2</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -2608,478 +4216,478 @@
         <v>32</v>
       </c>
       <c r="B52" s="2">
-        <v>0.30599999999999999</v>
+        <v>0.27400000000000002</v>
       </c>
       <c r="C52">
-        <v>4.9000000000000002E-2</v>
+        <v>-6.0999999999999999E-2</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="B53" s="2">
-        <v>0.28100000000000003</v>
+        <v>0.27300000000000002</v>
       </c>
       <c r="C53">
-        <v>4.8000000000000001E-2</v>
+        <v>-5.5E-2</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="B54" s="2">
-        <v>0.54</v>
+        <v>0.27100000000000002</v>
       </c>
       <c r="C54">
-        <v>4.8000000000000001E-2</v>
+        <v>-5.5E-2</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="B55" s="2">
-        <v>0.30499999999999999</v>
+        <v>0.27</v>
       </c>
       <c r="C55">
-        <v>3.6999999999999998E-2</v>
+        <v>-6.8000000000000005E-2</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="B56" s="2">
-        <v>0.28599999999999998</v>
+        <v>0.26800000000000002</v>
       </c>
       <c r="C56">
-        <v>3.5000000000000003E-2</v>
+        <v>-6.0999999999999999E-2</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="B57" s="2">
-        <v>0.314</v>
+        <v>0.25900000000000001</v>
       </c>
       <c r="C57">
-        <v>3.1E-2</v>
+        <v>-8.4000000000000005E-2</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="B58" s="2">
-        <v>0.51100000000000001</v>
+        <v>0.25800000000000001</v>
       </c>
       <c r="C58">
-        <v>2.3E-2</v>
+        <v>-3.9E-2</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>82</v>
+        <v>9</v>
       </c>
       <c r="B59" s="2">
-        <v>0.32400000000000001</v>
+        <v>0.252</v>
       </c>
       <c r="C59">
-        <v>2.3E-2</v>
+        <v>-4.7E-2</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="B60" s="2">
-        <v>0.34799999999999998</v>
+        <v>0.24299999999999999</v>
       </c>
       <c r="C60">
-        <v>2.1000000000000001E-2</v>
+        <v>-5.2999999999999999E-2</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="B61" s="2">
-        <v>0.371</v>
+        <v>0.24199999999999999</v>
       </c>
       <c r="C61">
-        <v>1.9E-2</v>
+        <v>-4.1000000000000002E-2</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A62" s="1" t="s">
-        <v>86</v>
+      <c r="A62" s="1">
+        <v>1</v>
       </c>
       <c r="B62" s="2">
-        <v>0.35099999999999998</v>
+        <v>0.23200000000000001</v>
       </c>
       <c r="C62">
-        <v>1.7000000000000001E-2</v>
+        <v>-1.9E-2</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B63" s="2">
-        <v>0.36</v>
+        <v>0.23100000000000001</v>
       </c>
       <c r="C63">
-        <v>1.4999999999999999E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="B64" s="2">
-        <v>0.32100000000000001</v>
+        <v>0.23100000000000001</v>
       </c>
       <c r="C64">
-        <v>1.4999999999999999E-2</v>
+        <v>-1.2E-2</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="B65" s="2">
-        <v>0.35699999999999998</v>
+        <v>0.23</v>
       </c>
       <c r="C65">
-        <v>1.4E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="B66" s="2">
-        <v>0.373</v>
+        <v>0.22800000000000001</v>
       </c>
       <c r="C66">
-        <v>1.4E-2</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" s="1" t="s">
-        <v>76</v>
+      <c r="A67" s="1">
+        <v>0</v>
       </c>
       <c r="B67" s="2">
-        <v>0.36399999999999999</v>
+        <v>0.224</v>
       </c>
       <c r="C67">
-        <v>1.2999999999999999E-2</v>
+        <v>-4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="B68" s="2">
-        <v>0.34499999999999997</v>
+        <v>0.222</v>
       </c>
       <c r="C68">
-        <v>1.2999999999999999E-2</v>
+        <v>-4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>4</v>
+        <v>89</v>
       </c>
       <c r="B69" s="2">
-        <v>0.37</v>
+        <v>0.22</v>
       </c>
       <c r="C69">
-        <v>1.2E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="B70" s="2">
-        <v>0.35799999999999998</v>
+        <v>0.214</v>
       </c>
       <c r="C70">
-        <v>1.2E-2</v>
+        <v>-1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B71" s="2">
-        <v>0.435</v>
+        <v>0.20699999999999999</v>
       </c>
       <c r="C71">
-        <v>1.2E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>83</v>
+        <v>13</v>
       </c>
       <c r="B72" s="2">
-        <v>0.35199999999999998</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="C72">
-        <v>1.0999999999999999E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="B73" s="2">
-        <v>0.43099999999999999</v>
+        <v>0.2</v>
       </c>
       <c r="C73">
-        <v>1.0999999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="B74" s="2">
-        <v>0.46</v>
+        <v>0.2</v>
       </c>
       <c r="C74">
-        <v>0.01</v>
+        <v>6.8000000000000005E-2</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="B75" s="2">
-        <v>0.35399999999999998</v>
+        <v>0.2</v>
       </c>
       <c r="C75">
-        <v>0.01</v>
+        <v>4.3999999999999997E-2</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
       <c r="B76" s="2">
-        <v>0.33300000000000002</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="C76">
-        <v>0.01</v>
+        <v>4.8000000000000001E-2</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A77" s="1">
-        <v>0</v>
+      <c r="A77" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="B77" s="2">
-        <v>0.35299999999999998</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="C77">
-        <v>8.9999999999999993E-3</v>
+        <v>4.9000000000000002E-2</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="B78" s="2">
-        <v>0.36699999999999999</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="C78">
-        <v>8.9999999999999993E-3</v>
+        <v>3.7999999999999999E-2</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="B79" s="2">
-        <v>0.36499999999999999</v>
+        <v>0.19500000000000001</v>
       </c>
       <c r="C79">
-        <v>8.9999999999999993E-3</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B80" s="2">
-        <v>0.47199999999999998</v>
+        <v>0.192</v>
       </c>
       <c r="C80">
-        <v>8.9999999999999993E-3</v>
+        <v>6.3E-2</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B81" s="2">
-        <v>0.46200000000000002</v>
+        <v>0.19</v>
       </c>
       <c r="C81">
-        <v>6.0000000000000001E-3</v>
+        <v>4.7E-2</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="B82" s="2">
-        <v>0.34100000000000003</v>
+        <v>0.182</v>
       </c>
       <c r="C82">
-        <v>5.0000000000000001E-3</v>
+        <v>9.0999999999999998E-2</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="B83" s="2">
-        <v>0.374</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="C83">
-        <v>4.0000000000000001E-3</v>
+        <v>6.7000000000000004E-2</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B84" s="2">
-        <v>0.38</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="C84">
-        <v>4.0000000000000001E-3</v>
+        <v>0.123</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B85" s="2">
-        <v>0.35599999999999998</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="C85">
-        <v>3.0000000000000001E-3</v>
+        <v>0.104</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="B86" s="2">
-        <v>0.33800000000000002</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="C86">
-        <v>3.0000000000000001E-3</v>
+        <v>7.5999999999999998E-2</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B87" s="2">
-        <v>0.36399999999999999</v>
+        <v>0.123</v>
       </c>
       <c r="C87">
-        <v>3.0000000000000001E-3</v>
+        <v>0.214</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B88" s="2">
-        <v>0.376</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="C88">
-        <v>3.0000000000000001E-3</v>
+        <v>0.26400000000000001</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="B89" s="2">
-        <v>0.46700000000000003</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="C89">
-        <v>1E-3</v>
+        <v>0.35199999999999998</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B90" s="2">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="C90">
         <v>0.40100000000000002</v>
-      </c>
-      <c r="C90">
-        <v>1E-3</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B91" s="2">
-        <v>0.378</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="C91">
-        <v>1E-3</v>
+        <v>0.441</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" s="1">
-        <v>1</v>
+      <c r="A92" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B92" s="2">
-        <v>0.40500000000000003</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>0.46400000000000002</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B93" s="2">
-        <v>0.45800000000000002</v>
-      </c>
-      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="C93" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B94" s="2">
-        <v>0.40200000000000002</v>
-      </c>
-      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="C94" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1">
     <sortState ref="A2:C94">
-      <sortCondition descending="1" ref="C1"/>
+      <sortCondition descending="1" ref="B1"/>
     </sortState>
   </autoFilter>
   <sortState ref="G13:I35">
@@ -3087,4 +4695,621 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:G31"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.1796875" customWidth="1"/>
+    <col min="4" max="6" width="12.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0.32</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="B7">
+        <v>0.36</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.31</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="B8">
+        <v>0.38</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.31</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="B9">
+        <v>0.4</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="B10">
+        <v>0.43</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.21</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="B11">
+        <v>0.44</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="B12">
+        <v>0.45</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="B13">
+        <v>0.48</v>
+      </c>
+      <c r="C13" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.41</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="B14">
+        <v>0.44</v>
+      </c>
+      <c r="C14" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.21</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="B15">
+        <v>0.44</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>0.46</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.34</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="4">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.34</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.39</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.21</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.39</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.41</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0.41</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="4">
+        <v>1</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.34</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.24</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>